<commit_message>
Updating Status for No PR found
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -324,12 +324,22 @@
   </si>
   <si>
     <t>EMEAAD\laroche</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,12 +394,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -420,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -437,6 +467,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,7 +752,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -726,33 +760,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
-    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="19.7109375" customWidth="1"/>
-    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,6 +886,9 @@
       <c r="AF1" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -950,6 +987,9 @@
       <c r="AF2" s="11" t="s">
         <v>40</v>
       </c>
+      <c r="AH2" t="s" s="12">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1048,6 +1088,9 @@
       <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="AH3" t="s" s="13">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1144,6 +1187,9 @@
       <c r="AF4" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="AH4" t="s" s="14">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1241,6 +1287,9 @@
       </c>
       <c r="AF5" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="AH5" t="s" s="15">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating organization select Condition || Common Method creation for viewDetails
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -179,9 +179,6 @@
     <t>STANDARD</t>
   </si>
   <si>
-    <t>EMEAAD\proch</t>
-  </si>
-  <si>
     <t>Approver3</t>
   </si>
   <si>
@@ -212,15 +209,9 @@
     <t>10</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>300</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>Aix  Golf</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>Purchase requisition</t>
   </si>
   <si>
-    <t>146</t>
-  </si>
-  <si>
     <t>136</t>
   </si>
   <si>
@@ -248,39 +236,15 @@
     <t>TEST_AUTO_OAR_08032022_01</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_02</t>
-  </si>
-  <si>
     <t>TEST_AUTO_OAR_08032022_03</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_04</t>
-  </si>
-  <si>
-    <t>Product2</t>
-  </si>
-  <si>
     <t>Product3</t>
   </si>
   <si>
-    <t>Product4</t>
-  </si>
-  <si>
-    <t>LOGISTICS</t>
-  </si>
-  <si>
-    <t>BUILDINGS MAINTENANCE</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Logistic</t>
-  </si>
-  <si>
-    <t>CP-AAST</t>
-  </si>
-  <si>
     <t>4290</t>
   </si>
   <si>
@@ -290,27 +254,9 @@
     <t>S00007077001</t>
   </si>
   <si>
-    <t>S00010321001</t>
-  </si>
-  <si>
     <t>Contractors</t>
   </si>
   <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>Auditor fees</t>
-  </si>
-  <si>
-    <t>S00010242001</t>
-  </si>
-  <si>
-    <t>4293</t>
-  </si>
-  <si>
-    <t>EMEAAD\dcoisplet</t>
-  </si>
-  <si>
     <t>190000</t>
   </si>
   <si>
@@ -318,28 +264,12 @@
   </si>
   <si>
     <t>EMEAAD\pbuisson</t>
-  </si>
-  <si>
-    <t>185000</t>
-  </si>
-  <si>
-    <t>EMEAAD\laroche</t>
-  </si>
-  <si>
-    <t>Test Status</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,32 +324,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -450,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -467,10 +377,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,41 +658,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="20" width="21.85546875" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="19.7109375" customWidth="1"/>
+    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -833,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>33</v>
@@ -884,10 +790,7 @@
         <v>27</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,10 +807,10 @@
         <v>21</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>26</v>
@@ -916,25 +819,25 @@
         <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>37</v>
@@ -943,52 +846,49 @@
         <v>36</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="AF2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" t="s" s="12">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1005,291 +905,86 @@
         <v>21</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>40</v>
+        <v>65</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH3" t="s" s="13">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH4" t="s" s="14">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH5" t="s" s="15">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1297,14 +992,12 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New Script for Pr creation without Approval
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F677BE8-FF20-4F86-B984-173DF3AD7F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13560"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -128,149 +120,159 @@
     <t>Agency/Site</t>
   </si>
   <si>
+    <t>Approver1</t>
+  </si>
+  <si>
+    <t>https://voflusoprasttest.p2p.basware.com</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Approver2</t>
+  </si>
+  <si>
+    <t>EMEAAD\anchaudhary</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Reviewer3</t>
+  </si>
+  <si>
+    <t>Reviewer2</t>
+  </si>
+  <si>
+    <t>Reviewer1</t>
+  </si>
+  <si>
+    <t>PRForm</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Approver3</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CP-APEX</t>
+  </si>
+  <si>
+    <t>EMEAAD\spineau</t>
+  </si>
+  <si>
+    <t>EMEAAD\msinno</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>Aix  Golf</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>docType</t>
+  </si>
+  <si>
+    <t>Purchase requisition</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>TEST_AUTO_OAR_08032022_03</t>
+  </si>
+  <si>
+    <t>Product3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4290</t>
+  </si>
+  <si>
+    <t>Contractors</t>
+  </si>
+  <si>
+    <t>190000</t>
+  </si>
+  <si>
+    <t>EMEAAD\esoyer</t>
+  </si>
+  <si>
+    <t>EMEAAD\pbuisson</t>
+  </si>
+  <si>
     <t>Provide2018</t>
   </si>
   <si>
-    <t>Approver1</t>
-  </si>
-  <si>
-    <t>https://voflusoprasttest.p2p.basware.com</t>
-  </si>
-  <si>
-    <t>ProductCode</t>
-  </si>
-  <si>
-    <t>SSP</t>
-  </si>
-  <si>
-    <t>Product1</t>
-  </si>
-  <si>
-    <t>Approver2</t>
-  </si>
-  <si>
-    <t>EMEAAD\anchaudhary</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Reviewer3</t>
-  </si>
-  <si>
-    <t>Reviewer2</t>
-  </si>
-  <si>
-    <t>Reviewer1</t>
-  </si>
-  <si>
-    <t>PRForm</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>STANDARD</t>
-  </si>
-  <si>
-    <t>Approver3</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CP-APEX</t>
-  </si>
-  <si>
-    <t>Catering for Seminar and Events</t>
-  </si>
-  <si>
-    <t>EMEAAD\spineau</t>
-  </si>
-  <si>
-    <t>EMEAAD\msinno</t>
-  </si>
-  <si>
-    <t>S00011626001</t>
-  </si>
-  <si>
-    <t>MAD</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>Aix  Golf</t>
-  </si>
-  <si>
-    <t>4993</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>docType</t>
-  </si>
-  <si>
-    <t>Purchase requisition</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>TEST_AUTO_OAR_08032022_01</t>
-  </si>
-  <si>
-    <t>TEST_AUTO_OAR_08032022_03</t>
-  </si>
-  <si>
-    <t>Product3</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4290</t>
-  </si>
-  <si>
-    <t>Subcontracting</t>
-  </si>
-  <si>
-    <t>S00007077001</t>
-  </si>
-  <si>
-    <t>Contractors</t>
-  </si>
-  <si>
-    <t>190000</t>
-  </si>
-  <si>
-    <t>EMEAAD\esoyer</t>
-  </si>
-  <si>
-    <t>EMEAAD\pbuisson</t>
+    <t>it</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>S00006372002</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 362 </t>
+  </si>
+  <si>
+    <t>HW - Network Security</t>
+  </si>
+  <si>
+    <t>S00000913001</t>
+  </si>
+  <si>
+    <t>C&amp;S SUB CONTRACTOR</t>
+  </si>
+  <si>
+    <t>4201</t>
+  </si>
+  <si>
+    <t>026909B2065</t>
+  </si>
+  <si>
+    <t>362</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,13 +325,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -360,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -377,6 +395,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -657,8 +678,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -666,36 +687,36 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
-    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="19.7109375" customWidth="1"/>
-    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="24" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -709,7 +730,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -718,7 +739,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
@@ -739,10 +760,10 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>6</v>
@@ -757,25 +778,25 @@
         <v>17</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>31</v>
@@ -784,214 +805,232 @@
         <v>30</v>
       </c>
       <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="AF2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s" s="13">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="6" t="s">
+    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="P3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="8"/>
+      <c r="V3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>60</v>
+      <c r="W3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="X3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>39</v>
+      <c r="Y3" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>65</v>
+        <v>36</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" t="s" s="14">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Test Data and Updating code for Approval
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F677BE8-FF20-4F86-B984-173DF3AD7F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F864A9E-E42D-4CE9-A71B-8EF94516E045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -78,9 +78,6 @@
     <t>PR tYPE</t>
   </si>
   <si>
-    <t>Nature</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -168,18 +165,6 @@
     <t/>
   </si>
   <si>
-    <t>CP-APEX</t>
-  </si>
-  <si>
-    <t>EMEAAD\spineau</t>
-  </si>
-  <si>
-    <t>EMEAAD\msinno</t>
-  </si>
-  <si>
-    <t>MAD</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -189,9 +174,6 @@
     <t>Aix  Golf</t>
   </si>
   <si>
-    <t>99</t>
-  </si>
-  <si>
     <t>docType</t>
   </si>
   <si>
@@ -201,48 +183,24 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_03</t>
-  </si>
-  <si>
     <t>Product3</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>4290</t>
-  </si>
-  <si>
-    <t>Contractors</t>
-  </si>
-  <si>
     <t>190000</t>
   </si>
   <si>
-    <t>EMEAAD\esoyer</t>
-  </si>
-  <si>
-    <t>EMEAAD\pbuisson</t>
-  </si>
-  <si>
-    <t>Provide2018</t>
-  </si>
-  <si>
     <t>it</t>
   </si>
   <si>
     <t>It</t>
   </si>
   <si>
-    <t>S00006372002</t>
-  </si>
-  <si>
     <t>Coding</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 362 </t>
-  </si>
-  <si>
     <t>HW - Network Security</t>
   </si>
   <si>
@@ -261,7 +219,31 @@
     <t>362</t>
   </si>
   <si>
+    <t>Test Automation India Anmol</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>Provide123*</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>S00008044001</t>
+  </si>
+  <si>
+    <t>Eur</t>
+  </si>
+  <si>
+    <t>EMEAAD\srofidal</t>
+  </si>
+  <si>
     <t>Test Status</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -332,12 +314,28 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -378,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -396,8 +394,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -679,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,45 +702,44 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="22.5703125" collapsed="false"/>
     <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
     <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
     <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="23" max="23" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="24" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
@@ -748,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>1</v>
@@ -757,273 +757,266 @@
         <v>2</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>8</v>
+      <c r="W1" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AE1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH2" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s" s="13">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="X3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="8"/>
-      <c r="V3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>44</v>
+      <c r="Y3" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI3" t="s" s="14">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH3" t="s" s="17">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Script for selling price
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F864A9E-E42D-4CE9-A71B-8EF94516E045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EDC4ED-07A5-418E-8807-BB2FB24C2C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -186,12 +186,6 @@
     <t>Product3</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>190000</t>
-  </si>
-  <si>
     <t>it</t>
   </si>
   <si>
@@ -240,13 +234,28 @@
     <t>EMEAAD\srofidal</t>
   </si>
   <si>
+    <t>EMEAAD\pvergez</t>
+  </si>
+  <si>
+    <t>EMEAAD\bcornu</t>
+  </si>
+  <si>
+    <t>SellingPrice</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
     <t>Test Status</t>
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -314,7 +323,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,7 +332,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,16 +350,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -376,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -394,11 +399,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -680,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,16 +713,16 @@
     <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
     <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
     <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="23" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -765,7 +771,7 @@
       <c r="P1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -778,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>7</v>
@@ -789,35 +795,38 @@
       <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" t="s">
-        <v>61</v>
+      <c r="AI1" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -828,13 +837,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>24</v>
@@ -843,10 +852,10 @@
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>35</v>
@@ -858,13 +867,13 @@
         <v>37</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>35</v>
@@ -879,19 +888,19 @@
         <v>35</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="Z2" s="6" t="s">
         <v>35</v>
@@ -899,26 +908,29 @@
       <c r="AA2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB2" s="13" t="s">
         <v>35</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH2" t="s" s="16">
-        <v>62</v>
+      <c r="AD2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI2" t="s" s="17">
+        <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -929,34 +941,34 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>41</v>
@@ -965,7 +977,7 @@
         <v>40</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="14" t="s">
         <v>35</v>
@@ -980,19 +992,19 @@
         <v>35</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="Z3" s="6" t="s">
         <v>35</v>
@@ -1001,22 +1013,25 @@
         <v>35</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="AC3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AD3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AE3" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="AF3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AH3" t="s" s="17">
-        <v>63</v>
+      <c r="AG3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI3" t="s" s="18">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed xpath for Supplier and Updated script for Po-Invoice
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,17 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EDC4ED-07A5-418E-8807-BB2FB24C2C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6457E45-9246-4888-914A-61CD00256A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -55,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -153,9 +163,6 @@
     <t>PRForm</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -165,12 +172,6 @@
     <t/>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>Aix  Golf</t>
   </si>
   <si>
@@ -195,67 +196,79 @@
     <t>Coding</t>
   </si>
   <si>
-    <t>HW - Network Security</t>
-  </si>
-  <si>
-    <t>S00000913001</t>
-  </si>
-  <si>
-    <t>C&amp;S SUB CONTRACTOR</t>
-  </si>
-  <si>
-    <t>4201</t>
-  </si>
-  <si>
     <t>026909B2065</t>
   </si>
   <si>
     <t>362</t>
   </si>
   <si>
-    <t>Test Automation India Anmol</t>
-  </si>
-  <si>
     <t>Product2</t>
   </si>
   <si>
     <t>Provide123*</t>
   </si>
   <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>S00008044001</t>
-  </si>
-  <si>
     <t>Eur</t>
   </si>
   <si>
     <t>EMEAAD\srofidal</t>
   </si>
   <si>
-    <t>EMEAAD\pvergez</t>
-  </si>
-  <si>
-    <t>EMEAAD\bcornu</t>
-  </si>
-  <si>
     <t>SellingPrice</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>1000</t>
+    <t>S00001610001</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>DSI-BUILD-OAR-50</t>
+  </si>
+  <si>
+    <t>DSI-BUILD-OAR-51</t>
+  </si>
+  <si>
+    <t>HW - Screen for PC</t>
+  </si>
+  <si>
+    <t>SW &amp; Solutions - IS-HR</t>
+  </si>
+  <si>
+    <t>RENT FIXED COST</t>
+  </si>
+  <si>
+    <t>SAAS FIXED COST</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>EMEAAD\lbaisin</t>
   </si>
   <si>
     <t>Test Status</t>
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -323,7 +336,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +363,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -404,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>31</v>
@@ -784,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>7</v>
@@ -796,7 +819,7 @@
         <v>23</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>17</v>
@@ -820,7 +843,7 @@
         <v>25</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI1" t="s">
         <v>65</v>
@@ -828,7 +851,7 @@
     </row>
     <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -837,13 +860,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>24</v>
@@ -852,79 +875,79 @@
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="J2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="O2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="T2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="8" t="s">
+      <c r="Y2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="AF2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AI2" t="s" s="17">
         <v>66</v>
@@ -932,7 +955,7 @@
     </row>
     <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
@@ -941,97 +964,97 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="N3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="T3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="8" t="s">
+      <c r="AC3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="AF3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AI3" t="s" s="18">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Log for Language of User
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6457E45-9246-4888-914A-61CD00256A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CA7635-AFCD-4FFB-859F-FD7D4DEA4C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>Auteur</author>
   </authors>
   <commentList>
     <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -45,7 +45,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Auteur:</t>
         </r>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="78">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -187,18 +187,9 @@
     <t>Product3</t>
   </si>
   <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>It</t>
-  </si>
-  <si>
     <t>Coding</t>
   </si>
   <si>
-    <t>026909B2065</t>
-  </si>
-  <si>
     <t>362</t>
   </si>
   <si>
@@ -235,12 +226,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>DSI-BUILD-OAR-50</t>
-  </si>
-  <si>
-    <t>DSI-BUILD-OAR-51</t>
-  </si>
-  <si>
     <t>HW - Screen for PC</t>
   </si>
   <si>
@@ -260,6 +245,51 @@
   </si>
   <si>
     <t>EMEAAD\lbaisin</t>
+  </si>
+  <si>
+    <t>[DSI-BUILD]-OAR-TEST CASE 5</t>
+  </si>
+  <si>
+    <t>[DSI-BUILD]-OAR-TEST CASE 6</t>
+  </si>
+  <si>
+    <t>413</t>
+  </si>
+  <si>
+    <t>[DSI-BUILD]-OAR-TEST CASE 7</t>
+  </si>
+  <si>
+    <t>Product4</t>
+  </si>
+  <si>
+    <t>[DSI-BUILD]-OAR-TEST CASE 8</t>
+  </si>
+  <si>
+    <t>Services - Hosting</t>
+  </si>
+  <si>
+    <t>S00010252001</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>TND</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>PAAS IAAS FIXED COST</t>
+  </si>
+  <si>
+    <t>EMEAAD\bcornu</t>
   </si>
   <si>
     <t>Test Status</t>
@@ -376,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -399,12 +429,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -426,11 +465,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,43 +751,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.44140625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.33203125" collapsed="false"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="22.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.88671875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.33203125" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.109375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.6640625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.6640625" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.6640625" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.88671875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.6640625" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.44140625" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="28.33203125" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="22.5546875" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5546875" collapsed="false"/>
     <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="20" max="21" customWidth="true" width="21.88671875" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.44140625" collapsed="false"/>
+    <col min="23" max="25" customWidth="true" style="1" width="15.88671875" collapsed="false"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="19.6640625" collapsed="false"/>
+    <col min="28" max="30" customWidth="true" width="19.6640625" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.109375" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.88671875" collapsed="false"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="17.5546875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -807,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>7</v>
@@ -819,7 +861,7 @@
         <v>23</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>17</v>
@@ -846,10 +888,10 @@
         <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -860,13 +902,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>24</v>
@@ -875,28 +917,28 @@
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>34</v>
@@ -911,19 +953,17 @@
         <v>34</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>43</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="X2" s="10"/>
       <c r="Y2" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Z2" s="6" t="s">
         <v>34</v>
@@ -941,7 +981,7 @@
         <v>34</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>34</v>
@@ -949,11 +989,11 @@
       <c r="AG2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" t="s" s="17">
-        <v>66</v>
+      <c r="AI2" t="s" s="18">
+        <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -964,34 +1004,34 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>38</v>
@@ -1000,7 +1040,7 @@
         <v>37</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="Q3" s="14" t="s">
         <v>34</v>
@@ -1015,46 +1055,246 @@
         <v>34</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="V3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI3" t="s" s="19">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="F4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI4" t="s" s="20">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB3" s="9" t="s">
+      <c r="E5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AC3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI3" t="s" s="18">
+      <c r="I5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>67</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI5" t="s" s="21">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1062,12 +1302,14 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C1B78C7E-7911-43ED-AF99-9E56177BCD8F}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{2C31F390-2496-4C99-ACCD-55C7E6D3A1AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix logs for better Analyze
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CA7635-AFCD-4FFB-859F-FD7D4DEA4C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216D2D0C-FBB0-4667-BE59-EE079E5ABD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -45,7 +44,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -145,9 +144,6 @@
     <t>Approver2</t>
   </si>
   <si>
-    <t>EMEAAD\anchaudhary</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -268,9 +264,6 @@
     <t>Services - Hosting</t>
   </si>
   <si>
-    <t>S00010252001</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -290,6 +283,12 @@
   </si>
   <si>
     <t>EMEAAD\bcornu</t>
+  </si>
+  <si>
+    <t>EMEAAD\oarsim</t>
+  </si>
+  <si>
+    <t>S00014700001</t>
   </si>
   <si>
     <t>Test Status</t>
@@ -472,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -754,40 +753,40 @@
   <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AH1" sqref="AH1:AN1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.44140625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.33203125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.88671875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.33203125" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.6640625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.6640625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.6640625" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.88671875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.6640625" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.44140625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="28.33203125" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="22.5546875" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="22.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
     <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="21" customWidth="true" width="21.88671875" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.44140625" collapsed="false"/>
-    <col min="23" max="25" customWidth="true" style="1" width="15.88671875" collapsed="false"/>
+    <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="23" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="19.6640625" collapsed="false"/>
-    <col min="28" max="30" customWidth="true" width="19.6640625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="23.109375" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.88671875" collapsed="false"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.5546875" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="33" max="33" customWidth="true" width="20.140625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -801,7 +800,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -831,10 +830,10 @@
         <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="16" t="s">
         <v>6</v>
@@ -849,7 +848,7 @@
         <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>7</v>
@@ -861,7 +860,7 @@
         <v>23</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>17</v>
@@ -870,13 +869,13 @@
         <v>18</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>20</v>
@@ -885,30 +884,30 @@
         <v>25</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>24</v>
@@ -917,381 +916,381 @@
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="T2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="X2" s="10"/>
       <c r="Y2" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI2" t="s" s="18">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="T3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="X3" s="10"/>
       <c r="Y3" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI3" t="s" s="19">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="I4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="M4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="N4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="T4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="V4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="X4" s="10"/>
       <c r="Y4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB4" s="9"/>
       <c r="AC4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AF4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI4" t="s" s="20">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="T5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="W5" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="X5" s="10"/>
       <c r="Y5" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AF5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI5" t="s" s="21">
         <v>77</v>

</xml_diff>

<commit_message>
Updating Full screenShot and Increase time for Edit Requisition And Update Logs
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216D2D0C-FBB0-4667-BE59-EE079E5ABD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584CF26D-6D6D-4709-84F9-532A4A2FE999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="3615" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -138,9 +138,6 @@
     <t>SSP</t>
   </si>
   <si>
-    <t>Product1</t>
-  </si>
-  <si>
     <t>Approver2</t>
   </si>
   <si>
@@ -177,60 +174,27 @@
     <t>Purchase requisition</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>Product3</t>
   </si>
   <si>
     <t>Coding</t>
   </si>
   <si>
-    <t>362</t>
-  </si>
-  <si>
-    <t>Product2</t>
-  </si>
-  <si>
     <t>Provide123*</t>
   </si>
   <si>
-    <t>Eur</t>
-  </si>
-  <si>
-    <t>EMEAAD\srofidal</t>
-  </si>
-  <si>
     <t>SellingPrice</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>S00001610001</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>HW - Screen for PC</t>
-  </si>
-  <si>
     <t>SW &amp; Solutions - IS-HR</t>
   </si>
   <si>
-    <t>RENT FIXED COST</t>
-  </si>
-  <si>
     <t>SAAS FIXED COST</t>
   </si>
   <si>
@@ -243,12 +207,6 @@
     <t>EMEAAD\lbaisin</t>
   </si>
   <si>
-    <t>[DSI-BUILD]-OAR-TEST CASE 5</t>
-  </si>
-  <si>
-    <t>[DSI-BUILD]-OAR-TEST CASE 6</t>
-  </si>
-  <si>
     <t>413</t>
   </si>
   <si>
@@ -292,9 +250,6 @@
   </si>
   <si>
     <t>Test Status</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -305,7 +260,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,12 +296,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
@@ -365,7 +314,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,16 +331,6 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
@@ -442,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -450,25 +389,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -750,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AN1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +705,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="22.5703125" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="13" width="22.5703125" collapsed="false"/>
     <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
     <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
     <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
@@ -800,7 +733,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -830,12 +763,12 @@
         <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -848,7 +781,7 @@
         <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>7</v>
@@ -860,7 +793,7 @@
         <v>23</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>17</v>
@@ -869,446 +802,240 @@
         <v>18</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="T2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="X2" s="10"/>
       <c r="Y2" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="AB2" s="9"/>
       <c r="AC2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI2" t="s" s="18">
-        <v>76</v>
+        <v>32</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI2" t="s" s="16">
+        <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="K3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="M3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="T3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="X3" s="10"/>
       <c r="Y3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="Z3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AC3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="AF3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI3" t="s" s="19">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" t="s" s="17">
         <v>62</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI4" t="s" s="20">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI5" t="s" s="21">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{C1B78C7E-7911-43ED-AF99-9E56177BCD8F}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{2C31F390-2496-4C99-ACCD-55C7E6D3A1AC}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C1B78C7E-7911-43ED-AF99-9E56177BCD8F}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{2C31F390-2496-4C99-ACCD-55C7E6D3A1AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scroll Testing for Elements
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A314B6-4485-4839-81A4-458F7BF6671F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED9DB5F-336F-4335-AD7B-541A5B66CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
     <t>Test Status</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -198,12 +198,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="42"/>
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="42"/>
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating Adding Line Data for purchase category,Imputation,Agency and ssp xpaths
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -162,7 +162,7 @@
     <t>Test Status</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -198,12 +198,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="10"/>
+        <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>

<commit_message>
updating Organization select method
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258E590D-64AA-4BCC-A6F5-38C300269D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60101181-0950-483B-8C0F-FCD395787DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -273,21 +273,41 @@
     <t>EMEAAD\pvergez</t>
   </si>
   <si>
-    <t>Test Status</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>362</t>
+  </si>
+  <si>
+    <t>[DSI-BUILD]-OAR-TEST CASE 5</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>HW - Screen for PC</t>
+  </si>
+  <si>
+    <t>S00001610001</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Eur</t>
+  </si>
+  <si>
+    <t>RENT FIXED COST</t>
+  </si>
+  <si>
+    <t>EMEAAD\srofidal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +366,14 @@
       <name val="Fira Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,26 +390,6 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>
@@ -424,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -454,8 +460,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -737,40 +756,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1:AJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="13" width="22.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="33" max="33" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="21" width="21.85546875" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="25" width="15.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="19.7109375" customWidth="1"/>
+    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -873,9 +892,6 @@
       <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -973,9 +989,6 @@
       <c r="AG2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" t="s" s="25">
-        <v>70</v>
-      </c>
     </row>
     <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1077,8 +1090,104 @@
       <c r="AG3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AI3" t="s" s="26">
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>71</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="V4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG4" s="32" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1086,12 +1195,13 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C1B78C7E-7911-43ED-AF99-9E56177BCD8F}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{08A1F94F-D207-4E1B-A1F4-653E7269FE7D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testing 413 and 010
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60101181-0950-483B-8C0F-FCD395787DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EF9AB3-9DFC-429C-A502-6EF6702DD98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -273,41 +273,18 @@
     <t>EMEAAD\pvergez</t>
   </si>
   <si>
-    <t>362</t>
-  </si>
-  <si>
-    <t>[DSI-BUILD]-OAR-TEST CASE 5</t>
-  </si>
-  <si>
-    <t>Product1</t>
-  </si>
-  <si>
-    <t>HW - Screen for PC</t>
-  </si>
-  <si>
-    <t>S00001610001</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>Eur</t>
-  </si>
-  <si>
-    <t>RENT FIXED COST</t>
-  </si>
-  <si>
-    <t>EMEAAD\srofidal</t>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,14 +343,8 @@
       <name val="Fira Sans"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +361,16 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -460,21 +441,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -756,40 +724,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AJ1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="21" width="21.85546875" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
-    <col min="23" max="25" width="15.85546875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="19.7109375" customWidth="1"/>
-    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="13" width="22.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="20" max="21" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="23" max="25" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="28" max="30" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="33" max="33" customWidth="true" width="20.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,6 +860,9 @@
       <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="AI1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -989,6 +960,9 @@
       <c r="AG2" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="AI2" t="s" s="25">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1090,104 +1064,8 @@
       <c r="AG3" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="25" t="s">
+      <c r="AI3" t="s" s="26">
         <v>70</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="O4" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="U4" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="V4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA4" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB4" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC4" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD4" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE4" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF4" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG4" s="32" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1195,13 +1073,12 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C1B78C7E-7911-43ED-AF99-9E56177BCD8F}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{08A1F94F-D207-4E1B-A1F4-653E7269FE7D}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Full Layout For Invoice
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -344,7 +347,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +374,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>
@@ -442,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1065,7 +1078,7 @@
         <v>32</v>
       </c>
       <c r="AI3" t="s" s="26">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating scroll into view for adding line purchase category
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7167EBB7-D3BE-4F42-BF11-5B6DA1FD6FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23E0D77-2317-451C-BADE-574993BBB966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>Environment</t>
   </si>
@@ -164,13 +164,49 @@
     <t>VEHI / MAINT / FIXED COST</t>
   </si>
   <si>
+    <t>EMEAAD\ehumbert</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>PO2213600592</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-001</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PO2213600593</t>
+  </si>
+  <si>
+    <t>S00000244002</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-002</t>
+  </si>
+  <si>
+    <t>PO2213600594</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-003</t>
+  </si>
+  <si>
     <t>ehumbert</t>
-  </si>
-  <si>
-    <t>EMEAAD\ehumbert</t>
-  </si>
-  <si>
-    <t>99</t>
   </si>
   <si>
     <t>Test Status</t>
@@ -255,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -299,6 +335,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
@@ -581,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,14 +730,16 @@
         <v>17</v>
       </c>
       <c r="AA1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="C2" s="13" t="s">
         <v>20</v>
       </c>
@@ -711,7 +752,9 @@
       <c r="F2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="H2" s="14" t="s">
         <v>25</v>
       </c>
@@ -719,60 +762,269 @@
         <v>36</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>35</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="R2" s="15" t="s">
         <v>31</v>
       </c>
       <c r="S2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA2" t="s" s="21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="16"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA3" t="s" s="22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="16"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4" t="s" s="23">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15" t="s">
+      <c r="T5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA2" t="s" s="21">
-        <v>46</v>
+      <c r="X5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" t="s" s="24">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{416163C3-617C-497E-AA3D-6E768404A1B6}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1EFBD0EA-5C5D-4D15-9193-570DDAA1D644}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{ACA9E775-FF4B-4CE5-B588-9AD7FD79CBB4}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{416163C3-617C-497E-AA3D-6E768404A1B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updating code for selsect Organization
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Environment</t>
   </si>
@@ -204,15 +204,6 @@
   </si>
   <si>
     <t>99</t>
-  </si>
-  <si>
-    <t>Test Status</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -245,32 +236,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -301,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -344,10 +315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -629,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -637,29 +604,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="33.85546875" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="11.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="8" width="26.28515625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="39.5703125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.5703125" collapsed="false"/>
-    <col min="14" max="14" style="6" width="9.140625" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.85546875" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="18" max="18" style="1" width="9.140625" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="30.7109375" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="19.85546875" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="6"/>
+    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -738,9 +705,6 @@
       <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -810,9 +774,6 @@
       <c r="Y2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" t="s" s="20">
-        <v>57</v>
-      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -880,9 +841,6 @@
       <c r="Y3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" t="s" s="21">
-        <v>57</v>
-      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -948,9 +906,6 @@
       <c r="Y4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AA4" t="s" s="22">
-        <v>57</v>
-      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1019,9 +974,6 @@
       </c>
       <c r="Y5" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="AA5" t="s" s="23">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solve problem of select all organization
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Environment</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>99</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -236,12 +242,22 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -272,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -315,6 +331,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -596,7 +616,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -604,29 +624,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="6"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="33.85546875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="21.140625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="8" width="26.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="39.5703125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="11.5703125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.5703125" collapsed="false"/>
+    <col min="14" max="14" style="6" width="9.140625" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.85546875" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="29.85546875" collapsed="false"/>
+    <col min="18" max="18" style="1" width="9.140625" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="30.7109375" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="19.85546875" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -705,6 +725,9 @@
       <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="AA1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -774,6 +797,9 @@
       <c r="Y2" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="AA2" t="s" s="20">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -841,6 +867,9 @@
       <c r="Y3" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="AA3" t="s" s="21">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -906,6 +935,9 @@
       <c r="Y4" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="AA4" t="s" s="22">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -974,6 +1006,9 @@
       </c>
       <c r="Y5" s="14" t="s">
         <v>23</v>
+      </c>
+      <c r="AA5" t="s" s="23">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>